<commit_message>
Updated version of document that includes summer 2020 field site data
</commit_message>
<xml_diff>
--- a/density_data/SUMPpnts_distance_area.xlsx
+++ b/density_data/SUMPpnts_distance_area.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamjohnson/Desktop/Laura/Hallett_Lab/Repositories/thesis-mussels/density_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC49270A-E83F-B24C-B21D-DB5677D70530}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB76EF91-AEB1-DD4C-B901-1EFE9A3FF566}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="660" windowWidth="28140" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,25 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="metadata" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="66">
   <si>
     <t>obs_id</t>
   </si>
@@ -178,7 +186,52 @@
     <t>area in square miles that drains to the site location. Derived from Streamstats basin delineation regression analysis.</t>
   </si>
   <si>
-    <t>ZERO_UmpConf</t>
+    <t>DAYSCH01</t>
+  </si>
+  <si>
+    <t>DAYSCH02</t>
+  </si>
+  <si>
+    <t>DAYSCH03</t>
+  </si>
+  <si>
+    <t>DAYSCH04</t>
+  </si>
+  <si>
+    <t>DAYSCH05</t>
+  </si>
+  <si>
+    <t>DAYSCH06</t>
+  </si>
+  <si>
+    <t>DAYSCH07</t>
+  </si>
+  <si>
+    <t>DAYSCH08</t>
+  </si>
+  <si>
+    <t>SR01</t>
+  </si>
+  <si>
+    <t>SR02</t>
+  </si>
+  <si>
+    <t>OB01</t>
+  </si>
+  <si>
+    <t>OB02</t>
+  </si>
+  <si>
+    <t>OB03</t>
+  </si>
+  <si>
+    <t>OB04</t>
+  </si>
+  <si>
+    <t>ZINCCMP01</t>
+  </si>
+  <si>
+    <t>ZINCCMP02</t>
   </si>
 </sst>
 </file>
@@ -196,7 +249,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -502,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -840,442 +893,694 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="1">
-        <v>158654.30234613625</v>
+        <v>129912.24</v>
       </c>
       <c r="D17" s="1">
-        <v>158.65430234613626</v>
-      </c>
-      <c r="E17" s="1">
-        <v>98.583182503121023</v>
-      </c>
-      <c r="F17" s="1">
-        <v>564</v>
-      </c>
+        <f>C17/1000</f>
+        <v>129.91224</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="1">
-        <v>79066.503306887185</v>
+        <v>129960.838</v>
       </c>
       <c r="D18" s="1">
-        <v>79.066503306887185</v>
-      </c>
-      <c r="E18" s="1">
-        <v>49.129632226303798</v>
-      </c>
-      <c r="F18" s="1">
-        <v>1410</v>
-      </c>
+        <f t="shared" ref="D18:D32" si="0">C18/1000</f>
+        <v>129.960838</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="1">
-        <v>113879.44178389855</v>
+        <v>129942.77099999999</v>
       </c>
       <c r="D19" s="1">
-        <v>113.87944178389856</v>
-      </c>
-      <c r="E19" s="1">
-        <v>70.761382620702832</v>
-      </c>
-      <c r="F19" s="1">
-        <v>699</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>129.94277099999999</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="1">
-        <v>158490.60965393484</v>
+        <v>129995.481</v>
       </c>
       <c r="D20" s="1">
-        <v>158.49060965393485</v>
-      </c>
-      <c r="E20" s="1">
-        <v>98.481468611275147</v>
-      </c>
-      <c r="F20" s="1">
-        <v>564</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>129.99548100000001</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="1">
-        <v>129974.94981455638</v>
+        <v>130182.427</v>
       </c>
       <c r="D21" s="1">
-        <v>129.9749498145564</v>
-      </c>
-      <c r="E21" s="1">
-        <v>80.762664541220715</v>
-      </c>
-      <c r="F21" s="1">
-        <v>643</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>130.18242699999999</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C22" s="1">
-        <v>129974.94981455638</v>
+        <v>130316.891</v>
       </c>
       <c r="D22" s="1">
-        <v>129.9749498145564</v>
-      </c>
-      <c r="E22" s="1">
-        <v>80.762664541220715</v>
-      </c>
-      <c r="F22" s="1">
-        <v>643</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>130.316891</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C23" s="1">
-        <v>137669.01243141145</v>
+        <v>130128.48699999999</v>
       </c>
       <c r="D23" s="1">
-        <v>137.66901243141146</v>
-      </c>
-      <c r="E23" s="1">
-        <v>85.543531923518572</v>
-      </c>
-      <c r="F23" s="1">
-        <v>630</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>130.12848700000001</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="1">
-        <v>39247.526389932493</v>
+        <v>130094.93</v>
       </c>
       <c r="D24" s="1">
-        <v>39.247526389932496</v>
-      </c>
-      <c r="E24" s="1">
-        <v>24.387274720438743</v>
-      </c>
-      <c r="F24" s="1">
-        <v>1640</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>130.09493000000001</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="1">
-        <v>39235.953918583808</v>
+        <v>157348.109</v>
       </c>
       <c r="D25" s="1">
-        <v>39.23595391858381</v>
-      </c>
-      <c r="E25" s="1">
-        <v>24.38008392234434</v>
-      </c>
-      <c r="F25" s="1">
-        <v>1640</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>157.34810899999999</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="1">
-        <v>73793.71406355458</v>
+        <v>157580.96599999999</v>
       </c>
       <c r="D26" s="1">
-        <v>73.793714063554589</v>
-      </c>
-      <c r="E26" s="1">
-        <v>45.853273901384973</v>
-      </c>
-      <c r="F26" s="1">
-        <v>1410</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>157.58096599999999</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="1">
-        <v>160095.24817083243</v>
+        <v>159871.80499999999</v>
       </c>
       <c r="D27" s="1">
-        <v>160.09524817083243</v>
-      </c>
-      <c r="E27" s="1">
-        <v>99.478544451158328</v>
-      </c>
-      <c r="F27" s="1">
-        <v>545</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>159.87180499999999</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="1">
-        <v>159827.60795750958</v>
+        <v>159945.03599999999</v>
       </c>
       <c r="D28" s="1">
-        <v>159.82760795750957</v>
-      </c>
-      <c r="E28" s="1">
-        <v>99.312240584165693</v>
-      </c>
-      <c r="F28" s="1">
-        <v>545</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>159.94503599999999</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C29" s="1">
-        <v>166877.09780876833</v>
+        <v>159984.503</v>
       </c>
       <c r="D29" s="1">
-        <v>166.87709780876833</v>
-      </c>
-      <c r="E29" s="1">
-        <v>103.69258914253219</v>
-      </c>
-      <c r="F29" s="1">
-        <v>451</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>159.98450299999999</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C30" s="1">
-        <v>157435.97869809557</v>
+        <v>160109.67300000001</v>
       </c>
       <c r="D30" s="1">
-        <v>157.43597869809557</v>
-      </c>
-      <c r="E30" s="1">
-        <v>97.826151519614342</v>
-      </c>
-      <c r="F30" s="1">
-        <v>565</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>160.10967300000002</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C31" s="1">
-        <v>173265.32358764537</v>
+        <v>196288.24299999999</v>
       </c>
       <c r="D31" s="1">
-        <v>173.26532358764538</v>
-      </c>
-      <c r="E31" s="1">
-        <v>107.6620473829788</v>
-      </c>
-      <c r="F31" s="1">
-        <v>441</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>196.28824299999999</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C32" s="1">
-        <v>70924.440120825282</v>
+        <v>196196.88800000001</v>
       </c>
       <c r="D32" s="1">
-        <v>70.924440120825281</v>
-      </c>
-      <c r="E32" s="1">
-        <v>44.070390282317327</v>
-      </c>
-      <c r="F32" s="1">
-        <v>1410</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>196.196888</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C33" s="1">
-        <v>36468.024718883717</v>
+        <v>158654.30234613625</v>
       </c>
       <c r="D33" s="1">
-        <v>36.468024718883719</v>
+        <v>158.65430234613626</v>
       </c>
       <c r="E33" s="1">
-        <v>22.660172987597495</v>
+        <v>98.583182503121023</v>
       </c>
       <c r="F33" s="1">
-        <v>474</v>
+        <v>564</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C34" s="1">
-        <v>36618.387372952697</v>
+        <v>79066.503306887185</v>
       </c>
       <c r="D34" s="1">
-        <v>36.618387372952697</v>
+        <v>79.066503306887185</v>
       </c>
       <c r="E34" s="1">
-        <v>22.753603980318992</v>
+        <v>49.129632226303798</v>
       </c>
       <c r="F34" s="1">
-        <v>474</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C35" s="1">
-        <v>37054.80273783172</v>
+        <v>113879.44178389855</v>
       </c>
       <c r="D35" s="1">
-        <v>37.054802737831722</v>
+        <v>113.87944178389856</v>
       </c>
       <c r="E35" s="1">
-        <v>23.024779832009234</v>
+        <v>70.761382620702832</v>
       </c>
       <c r="F35" s="1">
-        <v>474</v>
+        <v>699</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C36" s="1">
-        <v>36322.368584171185</v>
+        <v>158490.60965393484</v>
       </c>
       <c r="D36" s="1">
-        <v>36.322368584171187</v>
+        <v>158.49060965393485</v>
       </c>
       <c r="E36" s="1">
-        <v>22.569666489515033</v>
+        <v>98.481468611275147</v>
       </c>
       <c r="F36" s="1">
-        <v>474</v>
+        <v>564</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C37" s="1">
-        <v>45843.168603325073</v>
+        <v>129974.94981455638</v>
       </c>
       <c r="D37" s="1">
-        <v>45.843168603325076</v>
+        <v>129.9749498145564</v>
       </c>
       <c r="E37" s="1">
-        <v>28.485615518216704</v>
+        <v>80.762664541220715</v>
       </c>
       <c r="F37" s="1">
-        <v>394</v>
+        <v>643</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C38" s="1">
-        <v>402.48583400000001</v>
-      </c>
-      <c r="D38">
-        <v>0.40248583399999999</v>
-      </c>
-      <c r="E38">
-        <v>0.25009310253119998</v>
+        <v>129974.94981455638</v>
+      </c>
+      <c r="D38" s="1">
+        <v>129.9749498145564</v>
+      </c>
+      <c r="E38" s="1">
+        <v>80.762664541220715</v>
       </c>
       <c r="F38" s="1">
-        <v>1800</v>
+        <v>643</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="1">
+        <v>137669.01243141145</v>
+      </c>
+      <c r="D39" s="1">
+        <v>137.66901243141146</v>
+      </c>
+      <c r="E39" s="1">
+        <v>85.543531923518572</v>
+      </c>
+      <c r="F39" s="1">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="1">
+        <v>39247.526389932493</v>
+      </c>
+      <c r="D40" s="1">
+        <v>39.247526389932496</v>
+      </c>
+      <c r="E40" s="1">
+        <v>24.387274720438743</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="1">
+        <v>39235.953918583808</v>
+      </c>
+      <c r="D41" s="1">
+        <v>39.23595391858381</v>
+      </c>
+      <c r="E41" s="1">
+        <v>24.38008392234434</v>
+      </c>
+      <c r="F41" s="1">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="1">
+        <v>73793.71406355458</v>
+      </c>
+      <c r="D42" s="1">
+        <v>73.793714063554589</v>
+      </c>
+      <c r="E42" s="1">
+        <v>45.853273901384973</v>
+      </c>
+      <c r="F42" s="1">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="1">
+        <v>160095.24817083243</v>
+      </c>
+      <c r="D43" s="1">
+        <v>160.09524817083243</v>
+      </c>
+      <c r="E43" s="1">
+        <v>99.478544451158328</v>
+      </c>
+      <c r="F43" s="1">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" s="1">
+        <v>159827.60795750958</v>
+      </c>
+      <c r="D44" s="1">
+        <v>159.82760795750957</v>
+      </c>
+      <c r="E44" s="1">
+        <v>99.312240584165693</v>
+      </c>
+      <c r="F44" s="1">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="1">
+        <v>166877.09780876833</v>
+      </c>
+      <c r="D45" s="1">
+        <v>166.87709780876833</v>
+      </c>
+      <c r="E45" s="1">
+        <v>103.69258914253219</v>
+      </c>
+      <c r="F45" s="1">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="1">
+        <v>157435.97869809557</v>
+      </c>
+      <c r="D46" s="1">
+        <v>157.43597869809557</v>
+      </c>
+      <c r="E46" s="1">
+        <v>97.826151519614342</v>
+      </c>
+      <c r="F46" s="1">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" s="1">
+        <v>173265.32358764537</v>
+      </c>
+      <c r="D47" s="1">
+        <v>173.26532358764538</v>
+      </c>
+      <c r="E47" s="1">
+        <v>107.6620473829788</v>
+      </c>
+      <c r="F47" s="1">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" s="1">
+        <v>70924.440120825282</v>
+      </c>
+      <c r="D48" s="1">
+        <v>70.924440120825281</v>
+      </c>
+      <c r="E48" s="1">
+        <v>44.070390282317327</v>
+      </c>
+      <c r="F48" s="1">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" s="1">
+        <v>36468.024718883717</v>
+      </c>
+      <c r="D49" s="1">
+        <v>36.468024718883719</v>
+      </c>
+      <c r="E49" s="1">
+        <v>22.660172987597495</v>
+      </c>
+      <c r="F49" s="1">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C50" s="1">
+        <v>36618.387372952697</v>
+      </c>
+      <c r="D50" s="1">
+        <v>36.618387372952697</v>
+      </c>
+      <c r="E50" s="1">
+        <v>22.753603980318992</v>
+      </c>
+      <c r="F50" s="1">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C51" s="1">
+        <v>37054.80273783172</v>
+      </c>
+      <c r="D51" s="1">
+        <v>37.054802737831722</v>
+      </c>
+      <c r="E51" s="1">
+        <v>23.024779832009234</v>
+      </c>
+      <c r="F51" s="1">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" s="1">
+        <v>36322.368584171185</v>
+      </c>
+      <c r="D52" s="1">
+        <v>36.322368584171187</v>
+      </c>
+      <c r="E52" s="1">
+        <v>22.569666489515033</v>
+      </c>
+      <c r="F52" s="1">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C53" s="1">
+        <v>45843.168603325073</v>
+      </c>
+      <c r="D53" s="1">
+        <v>45.843168603325076</v>
+      </c>
+      <c r="E53" s="1">
+        <v>28.485615518216704</v>
+      </c>
+      <c r="F53" s="1">
+        <v>394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>